<commit_message>
Document Updates for 2024
</commit_message>
<xml_diff>
--- a/public/documents/kdl/KDL-Dead-Money-2024.xlsx
+++ b/public/documents/kdl/KDL-Dead-Money-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Corey\Documents\Fantasy Sports\KDL\2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHub\knuckleheads\public\documents\kdl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156C4FF4-FFAA-43C5-8698-F59CFE6D2DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1265B8-66DB-424C-85A8-7AB621E268F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39885" yWindow="1493" windowWidth="32212" windowHeight="17572" xr2:uid="{9DABBF3F-11D6-42CD-B88B-456B7A82B785}"/>
+    <workbookView xWindow="2475" yWindow="1312" windowWidth="33922" windowHeight="18571" xr2:uid="{9DABBF3F-11D6-42CD-B88B-456B7A82B785}"/>
   </bookViews>
   <sheets>
     <sheet name="Dead Money Summary" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="246">
   <si>
     <t>Franchise</t>
   </si>
@@ -782,13 +782,22 @@
     <t>Dead Money</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
     <t>Grand Total</t>
   </si>
   <si>
     <t>Sum of Dead Money</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Sum of Years</t>
+  </si>
+  <si>
+    <t>Sum of Salary</t>
+  </si>
+  <si>
+    <t>Fightin' Irish Mist Total</t>
   </si>
 </sst>
 </file>
@@ -830,10 +839,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,16 +872,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4767</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38104</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -910,7 +917,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4476750" y="304800"/>
+              <a:off x="10601325" y="519112"/>
               <a:ext cx="1828800" cy="2595567"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1132,10 +1139,50 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Salary" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="147"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="147" count="34">
+        <n v="4"/>
+        <n v="1"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="15"/>
+        <n v="3"/>
+        <n v="17"/>
+        <n v="9"/>
+        <n v="24"/>
+        <n v="7"/>
+        <n v="20"/>
+        <n v="2"/>
+        <n v="10"/>
+        <n v="16"/>
+        <n v="44"/>
+        <n v="37"/>
+        <n v="41"/>
+        <n v="8"/>
+        <n v="52"/>
+        <n v="110"/>
+        <n v="5"/>
+        <n v="29"/>
+        <n v="33"/>
+        <n v="18"/>
+        <n v="21"/>
+        <n v="147"/>
+        <n v="6"/>
+        <n v="28"/>
+        <n v="56"/>
+        <n v="13"/>
+        <n v="14"/>
+        <n v="25"/>
+        <n v="35"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Years" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="4">
+        <n v="1"/>
+        <n v="3"/>
+        <n v="2"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Date" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -1167,8 +1214,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="0"/>
-    <n v="4"/>
-    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="Thu Sep 7 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1176,8 +1223,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="1"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 7:34:39 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1185,8 +1232,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="2"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1194,8 +1241,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="3"/>
-    <n v="1"/>
-    <n v="3"/>
+    <x v="1"/>
+    <x v="1"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -1203,8 +1250,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="4"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1212,8 +1259,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="5"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1221,8 +1268,8 @@
     <x v="0"/>
     <n v="2"/>
     <x v="6"/>
-    <n v="11"/>
-    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1230,8 +1277,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="7"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1239,8 +1286,8 @@
     <x v="0"/>
     <n v="2"/>
     <x v="8"/>
-    <n v="12"/>
-    <n v="1"/>
+    <x v="3"/>
+    <x v="0"/>
     <s v="Wed Sep 27 8:09:15 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1248,8 +1295,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="9"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Wed Sep 27 8:09:27 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1257,8 +1304,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="10"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Oct 1 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1266,8 +1313,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="8"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Tue Oct 10 9:08:08 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1275,8 +1322,8 @@
     <x v="0"/>
     <n v="6"/>
     <x v="11"/>
-    <n v="15"/>
-    <n v="2"/>
+    <x v="4"/>
+    <x v="2"/>
     <s v="Thu Oct 12 11:15:12 a.m. ET 2023"/>
     <x v="2"/>
   </r>
@@ -1284,8 +1331,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="12"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1293,8 +1340,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="13"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1302,8 +1349,8 @@
     <x v="0"/>
     <n v="1"/>
     <x v="14"/>
-    <n v="3"/>
-    <n v="2"/>
+    <x v="5"/>
+    <x v="2"/>
     <s v="Sun Oct 22 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1311,8 +1358,8 @@
     <x v="0"/>
     <n v="3"/>
     <x v="15"/>
-    <n v="17"/>
-    <n v="1"/>
+    <x v="6"/>
+    <x v="0"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1320,8 +1367,8 @@
     <x v="0"/>
     <n v="1"/>
     <x v="16"/>
-    <n v="9"/>
-    <n v="1"/>
+    <x v="7"/>
+    <x v="0"/>
     <s v="Thu Nov 30 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1329,8 +1376,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="17"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 7 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1338,8 +1385,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="12"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 7 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1347,8 +1394,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="18"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1356,8 +1403,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="19"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1365,8 +1412,8 @@
     <x v="0"/>
     <n v="0"/>
     <x v="20"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1374,8 +1421,8 @@
     <x v="1"/>
     <n v="0"/>
     <x v="21"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1383,8 +1430,8 @@
     <x v="1"/>
     <n v="0"/>
     <x v="22"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Sun Nov 12 7:00:00 a.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1392,8 +1439,8 @@
     <x v="1"/>
     <n v="0"/>
     <x v="23"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Nov 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1401,8 +1448,8 @@
     <x v="2"/>
     <n v="0"/>
     <x v="24"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1410,8 +1457,8 @@
     <x v="2"/>
     <n v="9"/>
     <x v="25"/>
-    <n v="24"/>
-    <n v="2"/>
+    <x v="8"/>
+    <x v="2"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -1419,8 +1466,8 @@
     <x v="3"/>
     <n v="0"/>
     <x v="26"/>
-    <n v="4"/>
-    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="Sun Oct 1 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1428,8 +1475,8 @@
     <x v="3"/>
     <n v="2"/>
     <x v="27"/>
-    <n v="7"/>
-    <n v="2"/>
+    <x v="9"/>
+    <x v="2"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1437,8 +1484,8 @@
     <x v="3"/>
     <n v="0"/>
     <x v="28"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1446,8 +1493,8 @@
     <x v="3"/>
     <n v="4"/>
     <x v="29"/>
-    <n v="20"/>
-    <n v="1"/>
+    <x v="10"/>
+    <x v="0"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1455,8 +1502,8 @@
     <x v="3"/>
     <n v="0"/>
     <x v="30"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1464,8 +1511,8 @@
     <x v="3"/>
     <n v="0"/>
     <x v="31"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Thu Nov 30 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1473,8 +1520,8 @@
     <x v="3"/>
     <n v="0"/>
     <x v="32"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Dec 3 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1482,8 +1529,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="33"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sat Sep 9 3:21:24 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1491,8 +1538,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="34"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sat Sep 9 3:21:47 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1500,8 +1547,8 @@
     <x v="4"/>
     <n v="2"/>
     <x v="35"/>
-    <n v="12"/>
-    <n v="1"/>
+    <x v="3"/>
+    <x v="0"/>
     <s v="Sat Sep 9 3:28:48 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1509,8 +1556,8 @@
     <x v="4"/>
     <n v="2"/>
     <x v="36"/>
-    <n v="10"/>
-    <n v="1"/>
+    <x v="12"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1518,8 +1565,8 @@
     <x v="4"/>
     <n v="3"/>
     <x v="37"/>
-    <n v="16"/>
-    <n v="1"/>
+    <x v="13"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1527,8 +1574,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="38"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1536,8 +1583,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="39"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1545,8 +1592,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="40"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Tue Nov 21 1:06:31 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1554,8 +1601,8 @@
     <x v="4"/>
     <n v="0"/>
     <x v="18"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 23 9:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1563,8 +1610,8 @@
     <x v="5"/>
     <n v="8"/>
     <x v="41"/>
-    <n v="44"/>
-    <n v="1"/>
+    <x v="14"/>
+    <x v="0"/>
     <s v="Fri Aug 25 1:11:13 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1572,8 +1619,8 @@
     <x v="5"/>
     <n v="7"/>
     <x v="42"/>
-    <n v="37"/>
-    <n v="1"/>
+    <x v="15"/>
+    <x v="0"/>
     <s v="Fri Aug 25 1:12:12 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1581,8 +1628,8 @@
     <x v="5"/>
     <n v="1"/>
     <x v="43"/>
-    <n v="2"/>
-    <n v="3"/>
+    <x v="11"/>
+    <x v="1"/>
     <s v="Mon Sep 4 5:22:25 a.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -1590,8 +1637,8 @@
     <x v="5"/>
     <n v="8"/>
     <x v="44"/>
-    <n v="41"/>
-    <n v="1"/>
+    <x v="16"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1599,8 +1646,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="45"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Oct 8 7:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1608,8 +1655,8 @@
     <x v="5"/>
     <n v="3"/>
     <x v="46"/>
-    <n v="8"/>
-    <n v="2"/>
+    <x v="17"/>
+    <x v="2"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1617,8 +1664,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="47"/>
-    <n v="1"/>
-    <n v="3"/>
+    <x v="1"/>
+    <x v="1"/>
     <s v="Fri Oct 20 11:49:35 a.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -1626,8 +1673,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="48"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1635,8 +1682,8 @@
     <x v="5"/>
     <n v="1"/>
     <x v="49"/>
-    <n v="4"/>
-    <n v="2"/>
+    <x v="0"/>
+    <x v="2"/>
     <s v="Sun Oct 29 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1644,8 +1691,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="50"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1653,8 +1700,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="51"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Nov 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1662,8 +1709,8 @@
     <x v="5"/>
     <n v="14"/>
     <x v="52"/>
-    <n v="37"/>
-    <n v="2"/>
+    <x v="15"/>
+    <x v="2"/>
     <s v="Thu Dec 7 7:20:11 p.m. ET 2023"/>
     <x v="4"/>
   </r>
@@ -1671,8 +1718,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="53"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 7 7:20:11 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1680,8 +1727,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="54"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 7 7:23:37 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1689,8 +1736,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="55"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Thu Dec 7 7:26:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1698,8 +1745,8 @@
     <x v="5"/>
     <n v="10"/>
     <x v="56"/>
-    <n v="52"/>
-    <n v="1"/>
+    <x v="18"/>
+    <x v="0"/>
     <s v="Sat Dec 9 12:09:09 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1707,8 +1754,8 @@
     <x v="5"/>
     <n v="44"/>
     <x v="57"/>
-    <n v="110"/>
-    <n v="2"/>
+    <x v="19"/>
+    <x v="2"/>
     <s v="Sat Dec 9 12:09:45 p.m. ET 2023"/>
     <x v="5"/>
   </r>
@@ -1716,8 +1763,8 @@
     <x v="5"/>
     <n v="3"/>
     <x v="58"/>
-    <n v="15"/>
-    <n v="1"/>
+    <x v="4"/>
+    <x v="0"/>
     <s v="Sun Dec 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1725,8 +1772,8 @@
     <x v="5"/>
     <n v="0"/>
     <x v="50"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Sun Dec 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1734,8 +1781,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="59"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Sun Aug 27 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1743,8 +1790,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="60"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Sun Aug 27 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1752,8 +1799,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="61"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Sep 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1761,8 +1808,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="62"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Sep 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1770,8 +1817,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="63"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Sun Sep 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1779,8 +1826,8 @@
     <x v="6"/>
     <n v="1"/>
     <x v="64"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1788,8 +1835,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="65"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1797,8 +1844,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="50"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Sun Sep 17 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1806,8 +1853,8 @@
     <x v="6"/>
     <n v="5"/>
     <x v="66"/>
-    <n v="29"/>
-    <n v="1"/>
+    <x v="21"/>
+    <x v="0"/>
     <s v="Sun Sep 17 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1815,8 +1862,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="67"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1824,8 +1871,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="68"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1833,8 +1880,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="69"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1842,8 +1889,8 @@
     <x v="6"/>
     <n v="13"/>
     <x v="70"/>
-    <n v="33"/>
-    <n v="2"/>
+    <x v="22"/>
+    <x v="2"/>
     <s v="Sun Sep 24 12:00:00 p.m. ET 2023"/>
     <x v="6"/>
   </r>
@@ -1851,8 +1898,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="71"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Thu Sep 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1860,8 +1907,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="72"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Tue Oct 3 8:07:24 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1869,8 +1916,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="73"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1878,8 +1925,8 @@
     <x v="6"/>
     <n v="3"/>
     <x v="74"/>
-    <n v="18"/>
-    <n v="1"/>
+    <x v="23"/>
+    <x v="0"/>
     <s v="Sun Oct 8 7:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1887,8 +1934,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="75"/>
-    <n v="2"/>
-    <n v="2"/>
+    <x v="11"/>
+    <x v="2"/>
     <s v="Sun Oct 8 7:00:00 a.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1896,8 +1943,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="76"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Oct 12 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1905,8 +1952,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="77"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1914,8 +1961,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="78"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1923,8 +1970,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="79"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1932,8 +1979,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="80"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1941,8 +1988,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="81"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1950,8 +1997,8 @@
     <x v="6"/>
     <n v="3"/>
     <x v="82"/>
-    <n v="18"/>
-    <n v="1"/>
+    <x v="23"/>
+    <x v="0"/>
     <s v="Sun Oct 29 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1959,8 +2006,8 @@
     <x v="6"/>
     <n v="4"/>
     <x v="83"/>
-    <n v="11"/>
-    <n v="2"/>
+    <x v="2"/>
+    <x v="2"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="2"/>
   </r>
@@ -1968,8 +2015,8 @@
     <x v="6"/>
     <n v="1"/>
     <x v="84"/>
-    <n v="3"/>
-    <n v="2"/>
+    <x v="5"/>
+    <x v="2"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -1977,8 +2024,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="85"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1986,8 +2033,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="86"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Nov 9 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -1995,8 +2042,8 @@
     <x v="6"/>
     <n v="8"/>
     <x v="87"/>
-    <n v="21"/>
-    <n v="2"/>
+    <x v="24"/>
+    <x v="2"/>
     <s v="Sun Nov 12 7:00:00 a.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -2004,8 +2051,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="88"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2013,8 +2060,8 @@
     <x v="6"/>
     <n v="2"/>
     <x v="89"/>
-    <n v="11"/>
-    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2022,8 +2069,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="90"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Sat Nov 18 7:28:18 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2031,8 +2078,8 @@
     <x v="6"/>
     <n v="1"/>
     <x v="91"/>
-    <n v="7"/>
-    <n v="1"/>
+    <x v="9"/>
+    <x v="0"/>
     <s v="Thu Nov 23 9:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2040,8 +2087,8 @@
     <x v="6"/>
     <n v="1"/>
     <x v="92"/>
-    <n v="7"/>
-    <n v="1"/>
+    <x v="9"/>
+    <x v="0"/>
     <s v="Thu Nov 30 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2049,8 +2096,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="93"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Sun Dec 3 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2058,8 +2105,8 @@
     <x v="6"/>
     <n v="0"/>
     <x v="94"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Sun Dec 3 12:23:15 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2067,8 +2114,8 @@
     <x v="6"/>
     <n v="1"/>
     <x v="95"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Thu Dec 7 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2076,8 +2123,8 @@
     <x v="7"/>
     <n v="0"/>
     <x v="96"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2085,8 +2132,8 @@
     <x v="7"/>
     <n v="29"/>
     <x v="97"/>
-    <n v="147"/>
-    <n v="1"/>
+    <x v="25"/>
+    <x v="0"/>
     <s v="Thu Sep 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2094,8 +2141,8 @@
     <x v="7"/>
     <n v="0"/>
     <x v="92"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2103,8 +2150,8 @@
     <x v="7"/>
     <n v="0"/>
     <x v="98"/>
-    <n v="1"/>
-    <n v="3"/>
+    <x v="1"/>
+    <x v="1"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -2112,8 +2159,8 @@
     <x v="7"/>
     <n v="0"/>
     <x v="99"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 16 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2121,8 +2168,8 @@
     <x v="7"/>
     <n v="0"/>
     <x v="100"/>
-    <n v="4"/>
-    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="Thu Nov 30 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2130,8 +2177,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="101"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2139,8 +2186,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="102"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2148,8 +2195,8 @@
     <x v="8"/>
     <n v="6"/>
     <x v="103"/>
-    <n v="10"/>
-    <n v="3"/>
+    <x v="12"/>
+    <x v="1"/>
     <s v="Thu Sep 28 12:00:00 p.m. ET 2023"/>
     <x v="1"/>
   </r>
@@ -2157,8 +2204,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="104"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Sep 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2166,8 +2213,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="105"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2175,8 +2222,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="106"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 12 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2184,8 +2231,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="107"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2193,8 +2240,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="108"/>
-    <n v="21"/>
-    <n v="1"/>
+    <x v="24"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2202,8 +2249,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="109"/>
-    <n v="6"/>
-    <n v="1"/>
+    <x v="26"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2211,8 +2258,8 @@
     <x v="8"/>
     <n v="5"/>
     <x v="110"/>
-    <n v="28"/>
-    <n v="1"/>
+    <x v="27"/>
+    <x v="0"/>
     <s v="Sun Oct 22 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2220,8 +2267,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="111"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Oct 22 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2229,8 +2276,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="18"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Oct 22 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2238,8 +2285,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="112"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Wed Oct 25 2:28:16 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2247,8 +2294,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="113"/>
-    <n v="24"/>
-    <n v="1"/>
+    <x v="8"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2256,8 +2303,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="114"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Oct 26 2:43:05 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -2265,8 +2312,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="115"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Sun Oct 29 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2274,8 +2321,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="116"/>
-    <n v="9"/>
-    <n v="1"/>
+    <x v="7"/>
+    <x v="0"/>
     <s v="Sun Oct 29 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2283,8 +2330,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="117"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 2 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2292,8 +2339,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="118"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 2 3:38:25 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2301,8 +2348,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="119"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Sun Nov 5 7:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2310,8 +2357,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="120"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 9 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2319,8 +2366,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="121"/>
-    <n v="9"/>
-    <n v="1"/>
+    <x v="7"/>
+    <x v="0"/>
     <s v="Thu Nov 9 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2328,8 +2375,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="122"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Nov 9 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2337,8 +2384,8 @@
     <x v="8"/>
     <n v="11"/>
     <x v="123"/>
-    <n v="56"/>
-    <n v="1"/>
+    <x v="28"/>
+    <x v="0"/>
     <s v="Wed Nov 15 11:22:50 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2346,8 +2393,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="124"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Thu Nov 23 9:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2355,8 +2402,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="115"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Thu Dec 7 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2364,8 +2411,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="125"/>
-    <n v="21"/>
-    <n v="1"/>
+    <x v="24"/>
+    <x v="0"/>
     <s v="Thu Dec 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2373,8 +2420,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="91"/>
-    <n v="21"/>
-    <n v="1"/>
+    <x v="24"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2382,8 +2429,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="126"/>
-    <n v="21"/>
-    <n v="1"/>
+    <x v="24"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2391,8 +2438,8 @@
     <x v="8"/>
     <n v="2"/>
     <x v="127"/>
-    <n v="11"/>
-    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2400,8 +2447,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="128"/>
-    <n v="2"/>
-    <n v="1"/>
+    <x v="11"/>
+    <x v="0"/>
     <s v="Thu Dec 21 9:16:53 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2409,8 +2456,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="129"/>
-    <n v="24"/>
-    <n v="1"/>
+    <x v="8"/>
+    <x v="0"/>
     <s v="Sat Dec 23 11:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2418,8 +2465,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="130"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Sun Dec 24 9:36:15 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2427,8 +2474,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="131"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 28 11:32:51 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2436,8 +2483,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="132"/>
-    <n v="4"/>
-    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2445,8 +2492,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="133"/>
-    <n v="7"/>
-    <n v="1"/>
+    <x v="9"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2454,8 +2501,8 @@
     <x v="8"/>
     <n v="4"/>
     <x v="134"/>
-    <n v="21"/>
-    <n v="1"/>
+    <x v="24"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2463,8 +2510,8 @@
     <x v="8"/>
     <n v="1"/>
     <x v="135"/>
-    <n v="9"/>
-    <n v="1"/>
+    <x v="7"/>
+    <x v="0"/>
     <s v="Sat Dec 30 12:23:33 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2472,8 +2519,8 @@
     <x v="8"/>
     <n v="2"/>
     <x v="15"/>
-    <n v="13"/>
-    <n v="1"/>
+    <x v="29"/>
+    <x v="0"/>
     <s v="Sun Dec 31 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2481,8 +2528,8 @@
     <x v="8"/>
     <n v="0"/>
     <x v="122"/>
-    <n v="3"/>
-    <n v="1"/>
+    <x v="5"/>
+    <x v="0"/>
     <s v="Sun Dec 31 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2490,8 +2537,8 @@
     <x v="9"/>
     <n v="0"/>
     <x v="109"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Sun Nov 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2499,8 +2546,8 @@
     <x v="9"/>
     <n v="3"/>
     <x v="136"/>
-    <n v="17"/>
-    <n v="1"/>
+    <x v="6"/>
+    <x v="0"/>
     <s v="Sun Dec 10 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2508,8 +2555,8 @@
     <x v="10"/>
     <n v="0"/>
     <x v="137"/>
-    <n v="1"/>
-    <n v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -2517,8 +2564,8 @@
     <x v="10"/>
     <n v="0"/>
     <x v="138"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 14 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2526,8 +2573,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="139"/>
-    <n v="11"/>
-    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2535,8 +2582,8 @@
     <x v="10"/>
     <n v="0"/>
     <x v="140"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Sep 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2544,8 +2591,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="14"/>
-    <n v="6"/>
-    <n v="1"/>
+    <x v="26"/>
+    <x v="0"/>
     <s v="Thu Sep 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2553,8 +2600,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="141"/>
-    <n v="10"/>
-    <n v="1"/>
+    <x v="12"/>
+    <x v="0"/>
     <s v="Thu Oct 5 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2562,8 +2609,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="128"/>
-    <n v="5"/>
-    <n v="2"/>
+    <x v="20"/>
+    <x v="2"/>
     <s v="Sun Oct 8 7:00:00 a.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -2571,8 +2618,8 @@
     <x v="10"/>
     <n v="3"/>
     <x v="142"/>
-    <n v="9"/>
-    <n v="2"/>
+    <x v="7"/>
+    <x v="2"/>
     <s v="Thu Oct 12 12:00:00 p.m. ET 2023"/>
     <x v="3"/>
   </r>
@@ -2580,8 +2627,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="143"/>
-    <n v="6"/>
-    <n v="1"/>
+    <x v="26"/>
+    <x v="0"/>
     <s v="Sun Oct 15 7:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2589,8 +2636,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="144"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Thu Oct 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2598,8 +2645,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="145"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Sun Oct 22 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2607,8 +2654,8 @@
     <x v="10"/>
     <n v="0"/>
     <x v="146"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2616,8 +2663,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="23"/>
-    <n v="11"/>
-    <n v="1"/>
+    <x v="2"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2625,8 +2672,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="147"/>
-    <n v="14"/>
-    <n v="1"/>
+    <x v="30"/>
+    <x v="0"/>
     <s v="Thu Oct 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2634,8 +2681,8 @@
     <x v="10"/>
     <n v="5"/>
     <x v="148"/>
-    <n v="25"/>
-    <n v="1"/>
+    <x v="31"/>
+    <x v="0"/>
     <s v="Sun Nov 5 7:00:00 a.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2643,8 +2690,8 @@
     <x v="10"/>
     <n v="7"/>
     <x v="149"/>
-    <n v="35"/>
-    <n v="1"/>
+    <x v="32"/>
+    <x v="0"/>
     <s v="Wed Nov 15 6:27:33 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2652,8 +2699,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="150"/>
-    <n v="10"/>
-    <n v="1"/>
+    <x v="12"/>
+    <x v="0"/>
     <s v="Sun Nov 19 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2661,8 +2708,8 @@
     <x v="10"/>
     <n v="3"/>
     <x v="151"/>
-    <n v="15"/>
-    <n v="1"/>
+    <x v="4"/>
+    <x v="0"/>
     <s v="Sun Nov 26 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2670,8 +2717,8 @@
     <x v="10"/>
     <n v="5"/>
     <x v="152"/>
-    <n v="25"/>
-    <n v="1"/>
+    <x v="31"/>
+    <x v="0"/>
     <s v="Thu Nov 30 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2679,8 +2726,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="153"/>
-    <n v="7"/>
-    <n v="1"/>
+    <x v="9"/>
+    <x v="0"/>
     <s v="Thu Nov 30 4:46:32 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2688,8 +2735,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="154"/>
-    <n v="10"/>
-    <n v="1"/>
+    <x v="12"/>
+    <x v="0"/>
     <s v="Sun Dec 3 12:23:15 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2697,8 +2744,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="111"/>
-    <n v="12"/>
-    <n v="1"/>
+    <x v="3"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2706,8 +2753,8 @@
     <x v="10"/>
     <n v="1"/>
     <x v="155"/>
-    <n v="5"/>
-    <n v="1"/>
+    <x v="20"/>
+    <x v="0"/>
     <s v="Thu Dec 21 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2715,8 +2762,8 @@
     <x v="10"/>
     <n v="2"/>
     <x v="156"/>
-    <n v="12"/>
-    <n v="1"/>
+    <x v="3"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2724,8 +2771,8 @@
     <x v="10"/>
     <n v="0"/>
     <x v="73"/>
-    <n v="1"/>
-    <n v="1"/>
+    <x v="1"/>
+    <x v="0"/>
     <s v="Thu Dec 28 12:00:00 p.m. ET 2023"/>
     <x v="0"/>
   </r>
@@ -2733,8 +2780,8 @@
     <x v="11"/>
     <m/>
     <x v="157"/>
-    <m/>
-    <m/>
+    <x v="33"/>
+    <x v="3"/>
     <m/>
     <x v="7"/>
   </r>
@@ -2742,15 +2789,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7083DBC-841F-4251-A563-48E5D5F3D6C2}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7083DBC-841F-4251-A563-48E5D5F3D6C2}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:E16" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="13">
         <item sd="0" x="4"/>
         <item sd="0" x="5"/>
         <item sd="0" x="0"/>
-        <item sd="0" x="3"/>
+        <item x="3"/>
         <item sd="0" x="9"/>
         <item sd="0" x="7"/>
         <item sd="0" x="1"/>
@@ -2761,10 +2808,15 @@
         <item sd="0" x="11"/>
         <item t="default"/>
       </items>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
+          <x14:pivotField fillDownLabels="1"/>
+        </ext>
+      </extLst>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="159">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="158">
         <item x="52"/>
         <item x="23"/>
         <item x="64"/>
@@ -2923,13 +2975,57 @@
         <item x="156"/>
         <item x="50"/>
         <item x="157"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0" defaultSubtotal="0">
+      <items count="34">
+        <item x="1"/>
+        <item x="11"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="20"/>
+        <item x="26"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="7"/>
+        <item x="12"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="4"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="23"/>
+        <item x="10"/>
+        <item x="24"/>
+        <item x="8"/>
+        <item x="31"/>
+        <item x="27"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="32"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="14"/>
+        <item x="18"/>
+        <item x="28"/>
+        <item x="19"/>
+        <item x="25"/>
+        <item x="33"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" compact="0" outline="0" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" multipleItemSelectionAllowed="1" showAll="0">
+    <pivotField compact="0" outline="0" showAll="0"/>
+    <pivotField dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="9">
         <item h="1" x="0"/>
         <item x="3"/>
@@ -2947,7 +3043,7 @@
     <field x="0"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="12">
     <i>
       <x v="1"/>
     </i>
@@ -2955,6 +3051,13 @@
       <x v="2"/>
     </i>
     <i>
+      <x v="3"/>
+      <x v="52"/>
+    </i>
+    <i r="1">
+      <x v="83"/>
+    </i>
+    <i t="default">
       <x v="3"/>
     </i>
     <i>
@@ -2979,10 +3082,23 @@
       <x/>
     </i>
   </rowItems>
-  <colItems count="1">
-    <i/>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
   </colItems>
-  <dataFields count="1">
+  <dataFields count="3">
+    <dataField name="Sum of Salary" fld="3" baseField="0" baseItem="3" numFmtId="5"/>
+    <dataField name="Sum of Years" fld="4" baseField="0" baseItem="3"/>
     <dataField name="Sum of Dead Money" fld="6" baseField="0" baseItem="0" numFmtId="5"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -3374,113 +3490,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A126B6-C050-4F73-ACAD-82F072D2438E}">
-  <dimension ref="A3:B13"/>
+  <dimension ref="A3:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C3" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>244</v>
+      </c>
+      <c r="D4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="2">
+        <v>163</v>
+      </c>
+      <c r="D5" s="3">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="2">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="2">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="2">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15" s="2">
+        <v>74</v>
+      </c>
+      <c r="D15" s="3">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>240</v>
       </c>
-      <c r="B3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="3">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="B9" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B11" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B12" s="3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B13" s="3">
+      <c r="C16" s="2">
+        <v>316</v>
+      </c>
+      <c r="D16" s="3">
+        <v>63</v>
+      </c>
+      <c r="E16" s="2">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId3"/>
+        <x14:slicer r:id="rId4"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
Updates to KDL Docs
</commit_message>
<xml_diff>
--- a/public/documents/kdl/KDL-Dead-Money-2024.xlsx
+++ b/public/documents/kdl/KDL-Dead-Money-2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\GitHub\knuckleheads\public\documents\kdl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED1265B8-66DB-424C-85A8-7AB621E268F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7FFBD5-1101-4116-B4D0-08A361BF8FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2475" yWindow="1312" windowWidth="33922" windowHeight="18571" xr2:uid="{9DABBF3F-11D6-42CD-B88B-456B7A82B785}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="245">
   <si>
     <t>Franchise</t>
   </si>
@@ -795,9 +795,6 @@
   </si>
   <si>
     <t>Sum of Salary</t>
-  </si>
-  <si>
-    <t>Fightin' Irish Mist Total</t>
   </si>
 </sst>
 </file>
@@ -872,16 +869,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38104</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>147641</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
@@ -917,7 +914,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10601325" y="519112"/>
+              <a:off x="6891338" y="266699"/>
               <a:ext cx="1828800" cy="2595567"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2789,15 +2786,15 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7083DBC-841F-4251-A563-48E5D5F3D6C2}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:E16" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E7083DBC-841F-4251-A563-48E5D5F3D6C2}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
       <items count="13">
         <item sd="0" x="4"/>
         <item sd="0" x="5"/>
         <item sd="0" x="0"/>
-        <item x="3"/>
+        <item sd="0" x="3"/>
         <item sd="0" x="9"/>
         <item sd="0" x="7"/>
         <item sd="0" x="1"/>
@@ -3043,7 +3040,7 @@
     <field x="0"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="12">
+  <rowItems count="10">
     <i>
       <x v="1"/>
     </i>
@@ -3051,13 +3048,6 @@
       <x v="2"/>
     </i>
     <i>
-      <x v="3"/>
-      <x v="52"/>
-    </i>
-    <i r="1">
-      <x v="83"/>
-    </i>
-    <i t="default">
       <x v="3"/>
     </i>
     <i>
@@ -3490,16 +3480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34A126B6-C050-4F73-ACAD-82F072D2438E}">
-  <dimension ref="A3:E16"/>
+  <dimension ref="A3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="25.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
@@ -3559,145 +3549,111 @@
       <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
       <c r="C7" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D9" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>214</v>
       </c>
       <c r="C10" s="2">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3">
         <v>2</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="C12" s="2">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="D13" s="3">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>164</v>
+        <v>240</v>
       </c>
       <c r="C14" s="2">
-        <v>11</v>
+        <v>316</v>
       </c>
       <c r="D14" s="3">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="E14" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="2">
-        <v>74</v>
-      </c>
-      <c r="D15" s="3">
-        <v>18</v>
-      </c>
-      <c r="E15" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>240</v>
-      </c>
-      <c r="C16" s="2">
-        <v>316</v>
-      </c>
-      <c r="D16" s="3">
-        <v>63</v>
-      </c>
-      <c r="E16" s="2">
         <v>112</v>
       </c>
     </row>

</xml_diff>